<commit_message>
adding random forest and xgboosting
</commit_message>
<xml_diff>
--- a/R-NLP/appl_nrc.xlsx
+++ b/R-NLP/appl_nrc.xlsx
@@ -446,10 +446,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>44280.79166666667</v>
+        <v>44281.41666666667</v>
       </c>
       <c r="B2">
-        <v>-0.9503067567181898</v>
+        <v>-0.9503067567181896</v>
       </c>
       <c r="C2" s="3">
         <v>44281</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>44280.83333333333</v>
+        <v>44281.45833333333</v>
       </c>
       <c r="B3">
         <v>-1.018815318987103</v>
@@ -488,10 +488,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>44280.875</v>
+        <v>44281.5</v>
       </c>
       <c r="B4">
-        <v>-0.9555766461234899</v>
+        <v>-0.9555766461234898</v>
       </c>
       <c r="C4" s="3">
         <v>44281</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>44280.91666666667</v>
+        <v>44281.54166666667</v>
       </c>
       <c r="B5">
         <v>-1.200626503469998</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>44280.95833333333</v>
+        <v>44281.58333333333</v>
       </c>
       <c r="B6">
         <v>-1.200626503469998</v>
@@ -551,10 +551,10 @@
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>44281</v>
+        <v>44281.625</v>
       </c>
       <c r="B7">
-        <v>-1.126848051795781</v>
+        <v>-1.12684805179578</v>
       </c>
       <c r="C7" s="3">
         <v>44281</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>44281.04166666667</v>
+        <v>44281.66666666667</v>
       </c>
       <c r="B8">
         <v>-1.150562554119633</v>
@@ -593,10 +593,10 @@
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>44281.08333333333</v>
+        <v>44281.70833333333</v>
       </c>
       <c r="B9">
-        <v>-1.308659236278672</v>
+        <v>-1.308659236278671</v>
       </c>
       <c r="C9" s="3">
         <v>44281</v>
@@ -614,10 +614,10 @@
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>44281.125</v>
+        <v>44281.75</v>
       </c>
       <c r="B10">
-        <v>-1.163210288692357</v>
+        <v>-1.163210288692356</v>
       </c>
       <c r="C10" s="3">
         <v>44281</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>44281.16666666667</v>
+        <v>44281.79166666667</v>
       </c>
       <c r="B11">
         <v>-1.074149157742768</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>44281.20833333333</v>
+        <v>44281.83333333333</v>
       </c>
       <c r="B12">
         <v>-1.389025049709513</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>44281.25</v>
+        <v>44281.875</v>
       </c>
       <c r="B13">
         <v>-1.200626503469998</v>
@@ -788,10 +788,10 @@
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>44281.29166666667</v>
+        <v>44281.91666666667</v>
       </c>
       <c r="B14">
-        <v>-0.9081476414757811</v>
+        <v>-0.908147641475781</v>
       </c>
       <c r="C14" s="3">
         <v>44281</v>
@@ -839,10 +839,10 @@
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>44281.33333333333</v>
+        <v>44281.95833333333</v>
       </c>
       <c r="B15">
-        <v>-0.9028777520704772</v>
+        <v>-0.902877752070477</v>
       </c>
       <c r="C15" s="3">
         <v>44281</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>44281.375</v>
+        <v>44282</v>
       </c>
       <c r="B16">
-        <v>-0.9476718120155379</v>
+        <v>-0.9476718120155377</v>
       </c>
       <c r="C16" s="3">
         <v>44281</v>
@@ -941,10 +941,10 @@
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>44281.41666666667</v>
+        <v>44282.04166666667</v>
       </c>
       <c r="B17">
-        <v>-0.9371320332049375</v>
+        <v>-0.9371320332049374</v>
       </c>
       <c r="C17" s="3">
         <v>44281</v>
@@ -992,10 +992,10 @@
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>44281.45833333333</v>
+        <v>44282.08333333333</v>
       </c>
       <c r="B18">
-        <v>-0.9081476414757811</v>
+        <v>-0.908147641475781</v>
       </c>
       <c r="C18" s="3">
         <v>44281</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>44283.79166666667</v>
+        <v>44284.41666666667</v>
       </c>
       <c r="B19">
         <v>-1.121578162390477</v>
@@ -1094,10 +1094,10 @@
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>44283.83333333333</v>
+        <v>44284.45833333333</v>
       </c>
       <c r="B20">
-        <v>-1.068879268337468</v>
+        <v>-1.068879268337467</v>
       </c>
       <c r="C20" s="3">
         <v>44284</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>44283.875</v>
+        <v>44284.5</v>
       </c>
       <c r="B21">
         <v>-1.031990042500359</v>
@@ -1196,10 +1196,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>44283.91666666667</v>
+        <v>44284.54166666667</v>
       </c>
       <c r="B22">
-        <v>-0.9450368673128896</v>
+        <v>-0.9450368673128895</v>
       </c>
       <c r="C22" s="3">
         <v>44284</v>
@@ -1247,10 +1247,10 @@
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>44283.95833333333</v>
+        <v>44284.58333333333</v>
       </c>
       <c r="B23">
-        <v>-0.7895751298565032</v>
+        <v>-0.7895751298565031</v>
       </c>
       <c r="C23" s="3">
         <v>44284</v>
@@ -1298,10 +1298,10 @@
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>44284</v>
+        <v>44284.625</v>
       </c>
       <c r="B24">
-        <v>-0.7869401851538513</v>
+        <v>-0.7869401851538512</v>
       </c>
       <c r="C24" s="3">
         <v>44284</v>
@@ -1349,10 +1349,10 @@
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>44284.04166666667</v>
+        <v>44284.66666666667</v>
       </c>
       <c r="B25">
-        <v>-0.9318621437996336</v>
+        <v>-0.9318621437996335</v>
       </c>
       <c r="C25" s="3">
         <v>44284</v>
@@ -1400,10 +1400,10 @@
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>44284.08333333333</v>
+        <v>44284.70833333333</v>
       </c>
       <c r="B26">
-        <v>-0.904195224421805</v>
+        <v>-0.9041952244218049</v>
       </c>
       <c r="C26" s="3">
         <v>44284</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>44284.125</v>
+        <v>44284.75</v>
       </c>
       <c r="B27">
-        <v>-0.9871959825552984</v>
+        <v>-0.9871959825552983</v>
       </c>
       <c r="C27" s="3">
         <v>44284</v>
@@ -1502,10 +1502,10 @@
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>44284.16666666667</v>
+        <v>44284.79166666667</v>
       </c>
       <c r="B28">
-        <v>-0.8040673257210796</v>
+        <v>-0.8040673257210795</v>
       </c>
       <c r="C28" s="3">
         <v>44284</v>
@@ -1553,10 +1553,10 @@
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>44284.20833333333</v>
+        <v>44284.83333333333</v>
       </c>
       <c r="B29">
-        <v>-0.8620361091793926</v>
+        <v>-0.8620361091793924</v>
       </c>
       <c r="C29" s="3">
         <v>44284</v>
@@ -1604,10 +1604,10 @@
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>44284.25</v>
+        <v>44284.875</v>
       </c>
       <c r="B30">
-        <v>-0.7837782515106705</v>
+        <v>-0.7837782515106704</v>
       </c>
       <c r="C30" s="3">
         <v>44284</v>
@@ -1655,10 +1655,10 @@
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>44284.29166666667</v>
+        <v>44284.91666666667</v>
       </c>
       <c r="B31">
-        <v>-0.8607186368280685</v>
+        <v>-0.8607186368280684</v>
       </c>
       <c r="C31" s="3">
         <v>44284</v>
@@ -1706,10 +1706,10 @@
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <v>44284.33333333333</v>
+        <v>44284.95833333333</v>
       </c>
       <c r="B32">
-        <v>-0.8607186368280685</v>
+        <v>-0.8607186368280684</v>
       </c>
       <c r="C32" s="3">
         <v>44284</v>
@@ -1757,10 +1757,10 @@
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>44284.375</v>
+        <v>44285</v>
       </c>
       <c r="B33">
-        <v>-0.8791632497466246</v>
+        <v>-0.8791632497466245</v>
       </c>
       <c r="C33" s="3">
         <v>44284</v>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>44284.41666666667</v>
+        <v>44285.04166666667</v>
       </c>
       <c r="B34">
         <v>-0.8712584156386725</v>
@@ -1859,10 +1859,10 @@
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <v>44284.45833333333</v>
+        <v>44285.08333333333</v>
       </c>
       <c r="B35">
-        <v>-0.8607186368280685</v>
+        <v>-0.8607186368280684</v>
       </c>
       <c r="C35" s="3">
         <v>44284</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <v>44284.79166666667</v>
+        <v>44285.41666666667</v>
       </c>
       <c r="B36">
         <v>-1.147927609416985</v>
@@ -1961,7 +1961,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <v>44284.83333333333</v>
+        <v>44285.45833333333</v>
       </c>
       <c r="B37">
         <v>-1.045164766013611</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <v>44284.875</v>
+        <v>44285.5</v>
       </c>
       <c r="B38">
         <v>-1.08205399185072</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <v>44284.91666666667</v>
+        <v>44285.54166666667</v>
       </c>
       <c r="B39">
         <v>-1.142657720011685</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>44284.95833333333</v>
+        <v>44285.58333333333</v>
       </c>
       <c r="B40">
         <v>-1.142657720011685</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>44285</v>
+        <v>44285.625</v>
       </c>
       <c r="B41">
         <v>-1.200626503469998</v>
@@ -2216,7 +2216,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>44285.04166666667</v>
+        <v>44285.66666666667</v>
       </c>
       <c r="B42">
         <v>-1.456216139627106</v>
@@ -2267,10 +2267,10 @@
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>44285.08333333333</v>
+        <v>44285.70833333333</v>
       </c>
       <c r="B43">
-        <v>-1.254642869874335</v>
+        <v>-1.254642869874334</v>
       </c>
       <c r="C43" s="3">
         <v>44285</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <v>44285.125</v>
+        <v>44285.75</v>
       </c>
       <c r="B44">
         <v>-1.261230231630959</v>
@@ -2369,7 +2369,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <v>44285.16666666667</v>
+        <v>44285.79166666667</v>
       </c>
       <c r="B45">
         <v>-1.235934762485516</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <v>44285.20833333333</v>
+        <v>44285.83333333333</v>
       </c>
       <c r="B46">
         <v>-1.350554857050814</v>
@@ -2471,7 +2471,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <v>44285.25</v>
+        <v>44285.875</v>
       </c>
       <c r="B47">
         <v>-1.211166282280598</v>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <v>44285.29166666667</v>
+        <v>44285.91666666667</v>
       </c>
       <c r="B48">
         <v>-1.253325397523007</v>
@@ -2573,7 +2573,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <v>44285.33333333333</v>
+        <v>44285.95833333333</v>
       </c>
       <c r="B49">
         <v>-1.261230231630959</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <v>44285.375</v>
+        <v>44286</v>
       </c>
       <c r="B50">
         <v>-1.255960342225659</v>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <v>44285.41666666667</v>
+        <v>44286.04166666667</v>
       </c>
       <c r="B51">
         <v>-1.277039899846863</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <v>44285.45833333333</v>
+        <v>44286.08333333333</v>
       </c>
       <c r="B52">
         <v>-1.253325397523007</v>
@@ -2777,10 +2777,10 @@
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <v>44285.79166666667</v>
+        <v>44286.41666666667</v>
       </c>
       <c r="B53">
-        <v>-0.7948450192618034</v>
+        <v>-0.7948450192618033</v>
       </c>
       <c r="C53" s="3">
         <v>44286</v>
@@ -2828,10 +2828,10 @@
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <v>44285.83333333333</v>
+        <v>44286.45833333333</v>
       </c>
       <c r="B54">
-        <v>-0.8159245768830078</v>
+        <v>-0.8159245768830077</v>
       </c>
       <c r="C54" s="3">
         <v>44286</v>
@@ -2879,10 +2879,10 @@
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <v>44285.875</v>
+        <v>44286.5</v>
       </c>
       <c r="B55">
-        <v>-0.7395111805061424</v>
+        <v>-0.7395111805061423</v>
       </c>
       <c r="C55" s="3">
         <v>44286</v>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <v>44285.91666666667</v>
+        <v>44286.54166666667</v>
       </c>
       <c r="B56">
         <v>-0.7790353510458992</v>
@@ -2981,10 +2981,10 @@
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <v>44285.95833333333</v>
+        <v>44286.58333333333</v>
       </c>
       <c r="B57">
-        <v>-0.7421461252087906</v>
+        <v>-0.7421461252087905</v>
       </c>
       <c r="C57" s="3">
         <v>44286</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <v>44286</v>
+        <v>44286.625</v>
       </c>
       <c r="B58">
         <v>-0.7974799639644553</v>
@@ -3083,10 +3083,10 @@
     </row>
     <row r="59">
       <c r="A59" s="2">
-        <v>44286.04166666667</v>
+        <v>44286.66666666667</v>
       </c>
       <c r="B59">
-        <v>-0.4931438508083106</v>
+        <v>-0.4931438508083105</v>
       </c>
       <c r="C59" s="3">
         <v>44286</v>
@@ -3134,7 +3134,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2">
-        <v>44286.08333333333</v>
+        <v>44286.70833333333</v>
       </c>
       <c r="B60">
         <v>-0.4733817655384303</v>
@@ -3185,10 +3185,10 @@
     </row>
     <row r="61">
       <c r="A61" s="2">
-        <v>44286.125</v>
+        <v>44286.75</v>
       </c>
       <c r="B61">
-        <v>-0.3613966156757805</v>
+        <v>-0.3613966156757804</v>
       </c>
       <c r="C61" s="3">
         <v>44286</v>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="62">
       <c r="A62" s="2">
-        <v>44286.16666666667</v>
+        <v>44286.79166666667</v>
       </c>
       <c r="B62">
         <v>-0.391698479756261</v>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="63">
       <c r="A63" s="2">
-        <v>44286.20833333333</v>
+        <v>44286.83333333333</v>
       </c>
       <c r="B63">
         <v>-0.5010486849162626</v>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2">
-        <v>44286.25</v>
+        <v>44286.875</v>
       </c>
       <c r="B64">
         <v>-0.5234457148887911</v>
@@ -3389,7 +3389,7 @@
     </row>
     <row r="65">
       <c r="A65" s="2">
-        <v>44286.29166666667</v>
+        <v>44286.91666666667</v>
       </c>
       <c r="B65">
         <v>-0.6604628394266213</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="66">
       <c r="A66" s="2">
-        <v>44286.33333333333</v>
+        <v>44286.95833333333</v>
       </c>
       <c r="B66">
         <v>-0.6999870099663819</v>
@@ -3491,7 +3491,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2">
-        <v>44286.375</v>
+        <v>44287</v>
       </c>
       <c r="B67">
         <v>-0.6762725076425256</v>
@@ -3542,10 +3542,10 @@
     </row>
     <row r="68">
       <c r="A68" s="2">
-        <v>44286.41666666667</v>
+        <v>44287.04166666667</v>
       </c>
       <c r="B68">
-        <v>-0.6367483371027688</v>
+        <v>-0.6367483371027687</v>
       </c>
       <c r="C68" s="3">
         <v>44286</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="69">
       <c r="A69" s="2">
-        <v>44286.45833333333</v>
+        <v>44287.08333333333</v>
       </c>
       <c r="B69">
         <v>-0.6604628394266213</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2">
-        <v>44286.79166666667</v>
+        <v>44287.41666666667</v>
       </c>
       <c r="B70">
         <v>-0.2467765211104787</v>
@@ -3695,10 +3695,10 @@
     </row>
     <row r="71">
       <c r="A71" s="2">
-        <v>44286.83333333333</v>
+        <v>44287.45833333333</v>
       </c>
       <c r="B71">
-        <v>-0.3310947515952962</v>
+        <v>-0.3310947515952961</v>
       </c>
       <c r="C71" s="3">
         <v>44287</v>
@@ -3746,10 +3746,10 @@
     </row>
     <row r="72">
       <c r="A72" s="2">
-        <v>44286.875</v>
+        <v>44287.5</v>
       </c>
       <c r="B72">
-        <v>-0.328459806892648</v>
+        <v>-0.3284598068926479</v>
       </c>
       <c r="C72" s="3">
         <v>44287</v>
@@ -3797,7 +3797,7 @@
     </row>
     <row r="73">
       <c r="A73" s="2">
-        <v>44286.91666666667</v>
+        <v>44287.54166666667</v>
       </c>
       <c r="B73">
         <v>-0.325824862189996</v>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2">
-        <v>44286.95833333333</v>
+        <v>44287.58333333333</v>
       </c>
       <c r="B74">
         <v>-0.3021103598661397</v>
@@ -3899,7 +3899,7 @@
     </row>
     <row r="75">
       <c r="A75" s="2">
-        <v>44287</v>
+        <v>44287.625</v>
       </c>
       <c r="B75">
         <v>-0.2731259681369832</v>
@@ -3950,10 +3950,10 @@
     </row>
     <row r="76">
       <c r="A76" s="2">
-        <v>44287.04166666667</v>
+        <v>44287.66666666667</v>
       </c>
       <c r="B76">
-        <v>-0.3179200280820439</v>
+        <v>-0.3179200280820438</v>
       </c>
       <c r="C76" s="3">
         <v>44287</v>
@@ -4001,10 +4001,10 @@
     </row>
     <row r="77">
       <c r="A77" s="2">
-        <v>44287.08333333333</v>
+        <v>44287.70833333333</v>
       </c>
       <c r="B77">
-        <v>-0.3627140880271046</v>
+        <v>-0.3627140880271045</v>
       </c>
       <c r="C77" s="3">
         <v>44287</v>
@@ -4052,7 +4052,7 @@
     </row>
     <row r="78">
       <c r="A78" s="2">
-        <v>44287.125</v>
+        <v>44287.75</v>
       </c>
       <c r="B78">
         <v>-0.3429520027572243</v>
@@ -4103,10 +4103,10 @@
     </row>
     <row r="79">
       <c r="A79" s="2">
-        <v>44287.16666666667</v>
+        <v>44287.79166666667</v>
       </c>
       <c r="B79">
-        <v>-0.5247631872401153</v>
+        <v>-0.5247631872401152</v>
       </c>
       <c r="C79" s="3">
         <v>44287</v>
@@ -4154,7 +4154,7 @@
     </row>
     <row r="80">
       <c r="A80" s="2">
-        <v>44287.20833333333</v>
+        <v>44287.83333333333</v>
       </c>
       <c r="B80">
         <v>-0.4707468208357783</v>
@@ -4205,10 +4205,10 @@
     </row>
     <row r="81">
       <c r="A81" s="2">
-        <v>44287.25</v>
+        <v>44287.875</v>
       </c>
       <c r="B81">
-        <v>-0.5603349407258997</v>
+        <v>-0.5603349407258996</v>
       </c>
       <c r="C81" s="3">
         <v>44287</v>
@@ -4256,10 +4256,10 @@
     </row>
     <row r="82">
       <c r="A82" s="2">
-        <v>44287.29166666667</v>
+        <v>44287.91666666667</v>
       </c>
       <c r="B82">
-        <v>-0.4391274844039737</v>
+        <v>-0.4391274844039736</v>
       </c>
       <c r="C82" s="3">
         <v>44287</v>
@@ -4307,10 +4307,10 @@
     </row>
     <row r="83">
       <c r="A83" s="2">
-        <v>44287.33333333333</v>
+        <v>44287.95833333333</v>
       </c>
       <c r="B83">
-        <v>-0.4575720973225261</v>
+        <v>-0.457572097322526</v>
       </c>
       <c r="C83" s="3">
         <v>44287</v>
@@ -4358,10 +4358,10 @@
     </row>
     <row r="84">
       <c r="A84" s="2">
-        <v>44287.375</v>
+        <v>44288</v>
       </c>
       <c r="B84">
-        <v>-0.4417624291066219</v>
+        <v>-0.4417624291066218</v>
       </c>
       <c r="C84" s="3">
         <v>44287</v>
@@ -4409,10 +4409,10 @@
     </row>
     <row r="85">
       <c r="A85" s="2">
-        <v>44287.41666666667</v>
+        <v>44288.04166666667</v>
       </c>
       <c r="B85">
-        <v>-0.4443973738092739</v>
+        <v>-0.4443973738092738</v>
       </c>
       <c r="C85" s="3">
         <v>44287</v>
@@ -4460,7 +4460,7 @@
     </row>
     <row r="86">
       <c r="A86" s="2">
-        <v>44287.45833333333</v>
+        <v>44288.08333333333</v>
       </c>
       <c r="B86">
         <v>-0.4364925397013217</v>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="87">
       <c r="A87" s="2">
-        <v>44290.79166666667</v>
+        <v>44291.41666666667</v>
       </c>
       <c r="B87">
         <v>-0.394333424458913</v>
@@ -4562,10 +4562,10 @@
     </row>
     <row r="88">
       <c r="A88" s="2">
-        <v>44290.83333333333</v>
+        <v>44291.45833333333</v>
       </c>
       <c r="B88">
-        <v>-0.3758888115403569</v>
+        <v>-0.3758888115403568</v>
       </c>
       <c r="C88" s="3">
         <v>44291</v>
@@ -4613,10 +4613,10 @@
     </row>
     <row r="89">
       <c r="A89" s="2">
-        <v>44290.875</v>
+        <v>44291.5</v>
       </c>
       <c r="B89">
-        <v>-0.3310947515952962</v>
+        <v>-0.3310947515952961</v>
       </c>
       <c r="C89" s="3">
         <v>44291</v>
@@ -4664,10 +4664,10 @@
     </row>
     <row r="90">
       <c r="A90" s="2">
-        <v>44290.91666666667</v>
+        <v>44291.54166666667</v>
       </c>
       <c r="B90">
-        <v>-0.4206828714854175</v>
+        <v>-0.4206828714854174</v>
       </c>
       <c r="C90" s="3">
         <v>44291</v>
@@ -4715,10 +4715,10 @@
     </row>
     <row r="91">
       <c r="A91" s="2">
-        <v>44290.95833333333</v>
+        <v>44291.58333333333</v>
       </c>
       <c r="B91">
-        <v>-0.3310947515952962</v>
+        <v>-0.3310947515952961</v>
       </c>
       <c r="C91" s="3">
         <v>44291</v>
@@ -4766,10 +4766,10 @@
     </row>
     <row r="92">
       <c r="A92" s="2">
-        <v>44291</v>
+        <v>44291.625</v>
       </c>
       <c r="B92">
-        <v>-0.2362367422998747</v>
+        <v>-0.2362367422998746</v>
       </c>
       <c r="C92" s="3">
         <v>44291</v>
@@ -4817,7 +4817,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2">
-        <v>44291.04166666667</v>
+        <v>44291.66666666667</v>
       </c>
       <c r="B93">
         <v>0.118163320206631</v>
@@ -4868,10 +4868,10 @@
     </row>
     <row r="94">
       <c r="A94" s="2">
-        <v>44291.08333333333</v>
+        <v>44291.70833333333</v>
       </c>
       <c r="B94">
-        <v>0.08153758883978499</v>
+        <v>0.08153758883978497</v>
       </c>
       <c r="C94" s="3">
         <v>44291</v>
@@ -4919,10 +4919,10 @@
     </row>
     <row r="95">
       <c r="A95" s="2">
-        <v>44291.125</v>
+        <v>44291.75</v>
       </c>
       <c r="B95">
-        <v>0.3144667005540983</v>
+        <v>0.3144667005540982</v>
       </c>
       <c r="C95" s="3">
         <v>44291</v>
@@ -4970,7 +4970,7 @@
     </row>
     <row r="96">
       <c r="A96" s="2">
-        <v>44291.16666666667</v>
+        <v>44291.79166666667</v>
       </c>
       <c r="B96">
         <v>0.2638757622632085</v>
@@ -5021,10 +5021,10 @@
     </row>
     <row r="97">
       <c r="A97" s="2">
-        <v>44291.20833333333</v>
+        <v>44291.83333333333</v>
       </c>
       <c r="B97">
-        <v>0.3197365899594022</v>
+        <v>0.3197365899594021</v>
       </c>
       <c r="C97" s="3">
         <v>44291</v>
@@ -5072,7 +5072,7 @@
     </row>
     <row r="98">
       <c r="A98" s="2">
-        <v>44291.25</v>
+        <v>44291.875</v>
       </c>
       <c r="B98">
         <v>0.2301484700692808</v>
@@ -5123,7 +5123,7 @@
     </row>
     <row r="99">
       <c r="A99" s="2">
-        <v>44291.29166666667</v>
+        <v>44291.91666666667</v>
       </c>
       <c r="B99">
         <v>0.3276414240673542</v>
@@ -5174,10 +5174,10 @@
     </row>
     <row r="100">
       <c r="A100" s="2">
-        <v>44291.33333333333</v>
+        <v>44291.95833333333</v>
       </c>
       <c r="B100">
-        <v>0.4066897651468716</v>
+        <v>0.4066897651468715</v>
       </c>
       <c r="C100" s="3">
         <v>44291</v>
@@ -5225,10 +5225,10 @@
     </row>
     <row r="101">
       <c r="A101" s="2">
-        <v>44291.375</v>
+        <v>44292</v>
       </c>
       <c r="B101">
-        <v>0.4330392121733761</v>
+        <v>0.433039212173376</v>
       </c>
       <c r="C101" s="3">
         <v>44291</v>
@@ -5276,10 +5276,10 @@
     </row>
     <row r="102">
       <c r="A102" s="2">
-        <v>44291.41666666667</v>
+        <v>44292.04166666667</v>
       </c>
       <c r="B102">
-        <v>0.4330392121733761</v>
+        <v>0.433039212173376</v>
       </c>
       <c r="C102" s="3">
         <v>44291</v>
@@ -5327,7 +5327,7 @@
     </row>
     <row r="103">
       <c r="A103" s="2">
-        <v>44291.45833333333</v>
+        <v>44292.08333333333</v>
       </c>
       <c r="B103">
         <v>0.3276414240673542</v>
@@ -5378,7 +5378,7 @@
     </row>
     <row r="104">
       <c r="A104" s="2">
-        <v>44291.79166666667</v>
+        <v>44292.41666666667</v>
       </c>
       <c r="B104">
         <v>0.1721796866109679</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="105">
       <c r="A105" s="2">
-        <v>44291.83333333333</v>
+        <v>44292.45833333333</v>
       </c>
       <c r="B105">
         <v>0.2380533041772329</v>
@@ -5480,7 +5480,7 @@
     </row>
     <row r="106">
       <c r="A106" s="2">
-        <v>44291.875</v>
+        <v>44292.5</v>
       </c>
       <c r="B106">
         <v>0.2222436359613287</v>
@@ -5531,7 +5531,7 @@
     </row>
     <row r="107">
       <c r="A107" s="2">
-        <v>44291.91666666667</v>
+        <v>44292.54166666667</v>
       </c>
       <c r="B107">
         <v>0.2828473641222936</v>
@@ -5582,7 +5582,7 @@
     </row>
     <row r="108">
       <c r="A108" s="2">
-        <v>44291.95833333333</v>
+        <v>44292.58333333333</v>
       </c>
       <c r="B108">
         <v>0.4725633827131366</v>
@@ -5633,10 +5633,10 @@
     </row>
     <row r="109">
       <c r="A109" s="2">
-        <v>44292</v>
+        <v>44292.625</v>
       </c>
       <c r="B109">
-        <v>0.493642940334341</v>
+        <v>0.4936429403343409</v>
       </c>
       <c r="C109" s="3">
         <v>44292</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="110">
       <c r="A110" s="2">
-        <v>44292.04166666667</v>
+        <v>44292.66666666667</v>
       </c>
       <c r="B110">
         <v>0.4541187697945804</v>
@@ -5735,7 +5735,7 @@
     </row>
     <row r="111">
       <c r="A111" s="2">
-        <v>44292.08333333333</v>
+        <v>44292.70833333333</v>
       </c>
       <c r="B111">
         <v>0.5805961155218103</v>
@@ -5786,7 +5786,7 @@
     </row>
     <row r="112">
       <c r="A112" s="2">
-        <v>44292.125</v>
+        <v>44292.75</v>
       </c>
       <c r="B112">
         <v>0.4751983274157848</v>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="113">
       <c r="A113" s="2">
-        <v>44292.16666666667</v>
+        <v>44292.79166666667</v>
       </c>
       <c r="B113">
         <v>0.3192096010188695</v>
@@ -5888,10 +5888,10 @@
     </row>
     <row r="114">
       <c r="A114" s="2">
-        <v>44292.20833333333</v>
+        <v>44292.83333333333</v>
       </c>
       <c r="B114">
-        <v>0.4643950541349182</v>
+        <v>0.4643950541349181</v>
       </c>
       <c r="C114" s="3">
         <v>44292</v>
@@ -5939,10 +5939,10 @@
     </row>
     <row r="115">
       <c r="A115" s="2">
-        <v>44292.25</v>
+        <v>44292.875</v>
       </c>
       <c r="B115">
-        <v>0.4844206338750648</v>
+        <v>0.4844206338750647</v>
       </c>
       <c r="C115" s="3">
         <v>44292</v>
@@ -5990,10 +5990,10 @@
     </row>
     <row r="116">
       <c r="A116" s="2">
-        <v>44292.29166666667</v>
+        <v>44292.91666666667</v>
       </c>
       <c r="B116">
-        <v>0.4093247098495198</v>
+        <v>0.4093247098495197</v>
       </c>
       <c r="C116" s="3">
         <v>44292</v>
@@ -6041,10 +6041,10 @@
     </row>
     <row r="117">
       <c r="A117" s="2">
-        <v>44292.33333333333</v>
+        <v>44292.95833333333</v>
       </c>
       <c r="B117">
-        <v>0.4145945992548237</v>
+        <v>0.4145945992548236</v>
       </c>
       <c r="C117" s="3">
         <v>44292</v>
@@ -6092,10 +6092,10 @@
     </row>
     <row r="118">
       <c r="A118" s="2">
-        <v>44292.375</v>
+        <v>44293</v>
       </c>
       <c r="B118">
-        <v>0.4145945992548237</v>
+        <v>0.4145945992548236</v>
       </c>
       <c r="C118" s="3">
         <v>44292</v>
@@ -6143,10 +6143,10 @@
     </row>
     <row r="119">
       <c r="A119" s="2">
-        <v>44292.41666666667</v>
+        <v>44293.04166666667</v>
       </c>
       <c r="B119">
-        <v>0.4224994333627758</v>
+        <v>0.4224994333627757</v>
       </c>
       <c r="C119" s="3">
         <v>44292</v>
@@ -6194,10 +6194,10 @@
     </row>
     <row r="120">
       <c r="A120" s="2">
-        <v>44292.45833333333</v>
+        <v>44293.08333333333</v>
       </c>
       <c r="B120">
-        <v>0.4093247098495198</v>
+        <v>0.4093247098495197</v>
       </c>
       <c r="C120" s="3">
         <v>44292</v>
@@ -6245,7 +6245,7 @@
     </row>
     <row r="121">
       <c r="A121" s="2">
-        <v>44292.79166666667</v>
+        <v>44293.41666666667</v>
       </c>
       <c r="B121">
         <v>0.4119596545521717</v>
@@ -6296,7 +6296,7 @@
     </row>
     <row r="122">
       <c r="A122" s="2">
-        <v>44292.83333333333</v>
+        <v>44293.45833333333</v>
       </c>
       <c r="B122">
         <v>0.4541187697945804</v>
@@ -6347,10 +6347,10 @@
     </row>
     <row r="123">
       <c r="A123" s="2">
-        <v>44292.875</v>
+        <v>44293.5</v>
       </c>
       <c r="B123">
-        <v>0.4488488803892803</v>
+        <v>0.4488488803892802</v>
       </c>
       <c r="C123" s="3">
         <v>44293</v>
@@ -6398,10 +6398,10 @@
     </row>
     <row r="124">
       <c r="A124" s="2">
-        <v>44292.91666666667</v>
+        <v>44293.54166666667</v>
       </c>
       <c r="B124">
-        <v>0.4066897651468716</v>
+        <v>0.4066897651468715</v>
       </c>
       <c r="C124" s="3">
         <v>44293</v>
@@ -6449,10 +6449,10 @@
     </row>
     <row r="125">
       <c r="A125" s="2">
-        <v>44292.95833333333</v>
+        <v>44293.58333333333</v>
       </c>
       <c r="B125">
-        <v>0.4330392121733761</v>
+        <v>0.433039212173376</v>
       </c>
       <c r="C125" s="3">
         <v>44293</v>
@@ -6500,7 +6500,7 @@
     </row>
     <row r="126">
       <c r="A126" s="2">
-        <v>44293</v>
+        <v>44293.625</v>
       </c>
       <c r="B126">
         <v>0.3065618664461461</v>
@@ -6551,10 +6551,10 @@
     </row>
     <row r="127">
       <c r="A127" s="2">
-        <v>44293.04166666667</v>
+        <v>44293.66666666667</v>
       </c>
       <c r="B127">
-        <v>0.6622794013039797</v>
+        <v>0.6622794013039796</v>
       </c>
       <c r="C127" s="3">
         <v>44293</v>
@@ -6602,10 +6602,10 @@
     </row>
     <row r="128">
       <c r="A128" s="2">
-        <v>44293.08333333333</v>
+        <v>44293.70833333333</v>
       </c>
       <c r="B128">
-        <v>0.6733461690551126</v>
+        <v>0.6733461690551125</v>
       </c>
       <c r="C128" s="3">
         <v>44293</v>
@@ -6653,7 +6653,7 @@
     </row>
     <row r="129">
       <c r="A129" s="2">
-        <v>44293.125</v>
+        <v>44293.75</v>
       </c>
       <c r="B129">
         <v>0.6512126335528466</v>
@@ -6704,7 +6704,7 @@
     </row>
     <row r="130">
       <c r="A130" s="2">
-        <v>44293.16666666667</v>
+        <v>44293.79166666667</v>
       </c>
       <c r="B130">
         <v>0.6306600648721712</v>
@@ -6755,10 +6755,10 @@
     </row>
     <row r="131">
       <c r="A131" s="2">
-        <v>44293.20833333333</v>
+        <v>44293.83333333333</v>
       </c>
       <c r="B131">
-        <v>0.811153777003738</v>
+        <v>0.8111537770037379</v>
       </c>
       <c r="C131" s="3">
         <v>44293</v>
@@ -6806,10 +6806,10 @@
     </row>
     <row r="132">
       <c r="A132" s="2">
-        <v>44293.25</v>
+        <v>44293.875</v>
       </c>
       <c r="B132">
-        <v>0.7018035718437364</v>
+        <v>0.7018035718437363</v>
       </c>
       <c r="C132" s="3">
         <v>44293</v>
@@ -6857,10 +6857,10 @@
     </row>
     <row r="133">
       <c r="A133" s="2">
-        <v>44293.29166666667</v>
+        <v>44293.91666666667</v>
       </c>
       <c r="B133">
-        <v>0.8546303645974747</v>
+        <v>0.8546303645974745</v>
       </c>
       <c r="C133" s="3">
         <v>44293</v>
@@ -6908,10 +6908,10 @@
     </row>
     <row r="134">
       <c r="A134" s="2">
-        <v>44293.33333333333</v>
+        <v>44293.95833333333</v>
       </c>
       <c r="B134">
-        <v>0.9073292586504836</v>
+        <v>0.9073292586504835</v>
       </c>
       <c r="C134" s="3">
         <v>44293</v>
@@ -6959,10 +6959,10 @@
     </row>
     <row r="135">
       <c r="A135" s="2">
-        <v>44293.375</v>
+        <v>44294</v>
       </c>
       <c r="B135">
-        <v>0.9125991480557876</v>
+        <v>0.9125991480557875</v>
       </c>
       <c r="C135" s="3">
         <v>44293</v>
@@ -7010,10 +7010,10 @@
     </row>
     <row r="136">
       <c r="A136" s="2">
-        <v>44293.41666666667</v>
+        <v>44294.04166666667</v>
       </c>
       <c r="B136">
-        <v>0.9389485950822921</v>
+        <v>0.938948595082292</v>
       </c>
       <c r="C136" s="3">
         <v>44293</v>
@@ -7061,10 +7061,10 @@
     </row>
     <row r="137">
       <c r="A137" s="2">
-        <v>44293.45833333333</v>
+        <v>44294.08333333333</v>
       </c>
       <c r="B137">
-        <v>0.8546303645974747</v>
+        <v>0.8546303645974745</v>
       </c>
       <c r="C137" s="3">
         <v>44293</v>
@@ -7112,10 +7112,10 @@
     </row>
     <row r="138">
       <c r="A138" s="2">
-        <v>44293.79166666667</v>
+        <v>44294.41666666667</v>
       </c>
       <c r="B138">
-        <v>1.089140443133375</v>
+        <v>1.089140443133374</v>
       </c>
       <c r="C138" s="3">
         <v>44294</v>
@@ -7163,7 +7163,7 @@
     </row>
     <row r="139">
       <c r="A139" s="2">
-        <v>44293.83333333333</v>
+        <v>44294.45833333333</v>
       </c>
       <c r="B139">
         <v>1.012727046756509</v>
@@ -7214,7 +7214,7 @@
     </row>
     <row r="140">
       <c r="A140" s="2">
-        <v>44293.875</v>
+        <v>44294.5</v>
       </c>
       <c r="B140">
         <v>1.1839984524288</v>
@@ -7265,7 +7265,7 @@
     </row>
     <row r="141">
       <c r="A141" s="2">
-        <v>44293.91666666667</v>
+        <v>44294.54166666667</v>
       </c>
       <c r="B141">
         <v>1.118124834862535</v>
@@ -7316,7 +7316,7 @@
     </row>
     <row r="142">
       <c r="A142" s="2">
-        <v>44293.95833333333</v>
+        <v>44294.58333333333</v>
       </c>
       <c r="B142">
         <v>1.099680221943982</v>
@@ -7367,7 +7367,7 @@
     </row>
     <row r="143">
       <c r="A143" s="2">
-        <v>44294</v>
+        <v>44294.625</v>
       </c>
       <c r="B143">
         <v>1.133934503078439</v>
@@ -7418,7 +7418,7 @@
     </row>
     <row r="144">
       <c r="A144" s="2">
-        <v>44294.04166666667</v>
+        <v>44294.66666666667</v>
       </c>
       <c r="B144">
         <v>1.226948051082</v>
@@ -7469,7 +7469,7 @@
     </row>
     <row r="145">
       <c r="A145" s="2">
-        <v>44294.08333333333</v>
+        <v>44294.70833333333</v>
       </c>
       <c r="B145">
         <v>1.276221517021569</v>
@@ -7520,7 +7520,7 @@
     </row>
     <row r="146">
       <c r="A146" s="2">
-        <v>44294.125</v>
+        <v>44294.75</v>
       </c>
       <c r="B146">
         <v>1.339460189885186</v>
@@ -7571,7 +7571,7 @@
     </row>
     <row r="147">
       <c r="A147" s="2">
-        <v>44294.16666666667</v>
+        <v>44294.79166666667</v>
       </c>
       <c r="B147">
         <v>1.4185085309647</v>
@@ -7622,7 +7622,7 @@
     </row>
     <row r="148">
       <c r="A148" s="2">
-        <v>44294.20833333333</v>
+        <v>44294.83333333333</v>
       </c>
       <c r="B148">
         <v>1.456715229153136</v>
@@ -7673,7 +7673,7 @@
     </row>
     <row r="149">
       <c r="A149" s="2">
-        <v>44294.25</v>
+        <v>44294.875</v>
       </c>
       <c r="B149">
         <v>1.414556113910727</v>
@@ -7724,7 +7724,7 @@
     </row>
     <row r="150">
       <c r="A150" s="2">
-        <v>44294.29166666667</v>
+        <v>44294.91666666667</v>
       </c>
       <c r="B150">
         <v>1.502826761449525</v>
@@ -7775,7 +7775,7 @@
     </row>
     <row r="151">
       <c r="A151" s="2">
-        <v>44294.33333333333</v>
+        <v>44294.95833333333</v>
       </c>
       <c r="B151">
         <v>1.57924015782639</v>
@@ -7826,7 +7826,7 @@
     </row>
     <row r="152">
       <c r="A152" s="2">
-        <v>44294.375</v>
+        <v>44295</v>
       </c>
       <c r="B152">
         <v>1.595049826042294</v>
@@ -7877,7 +7877,7 @@
     </row>
     <row r="153">
       <c r="A153" s="2">
-        <v>44294.41666666667</v>
+        <v>44295.04166666667</v>
       </c>
       <c r="B153">
         <v>1.56870037901579</v>
@@ -7928,7 +7928,7 @@
     </row>
     <row r="154">
       <c r="A154" s="2">
-        <v>44294.45833333333</v>
+        <v>44295.08333333333</v>
       </c>
       <c r="B154">
         <v>1.502826761449525</v>
@@ -7979,7 +7979,7 @@
     </row>
     <row r="155">
       <c r="A155" s="2">
-        <v>44294.79166666667</v>
+        <v>44295.41666666667</v>
       </c>
       <c r="B155">
         <v>1.4185085309647</v>
@@ -8030,10 +8030,10 @@
     </row>
     <row r="156">
       <c r="A156" s="2">
-        <v>44294.83333333333</v>
+        <v>44295.45833333333</v>
       </c>
       <c r="B156">
-        <v>1.4079687521541</v>
+        <v>1.407968752154099</v>
       </c>
       <c r="C156" s="3">
         <v>44295</v>
@@ -8081,7 +8081,7 @@
     </row>
     <row r="157">
       <c r="A157" s="2">
-        <v>44294.875</v>
+        <v>44295.5</v>
       </c>
       <c r="B157">
         <v>1.321015576966626</v>
@@ -8132,7 +8132,7 @@
     </row>
     <row r="158">
       <c r="A158" s="2">
-        <v>44294.91666666667</v>
+        <v>44295.54166666667</v>
       </c>
       <c r="B158">
         <v>1.457769207034194</v>
@@ -8183,7 +8183,7 @@
     </row>
     <row r="159">
       <c r="A159" s="2">
-        <v>44294.95833333333</v>
+        <v>44295.58333333333</v>
       </c>
       <c r="B159">
         <v>1.378984360424939</v>
@@ -8234,7 +8234,7 @@
     </row>
     <row r="160">
       <c r="A160" s="2">
-        <v>44295</v>
+        <v>44295.625</v>
       </c>
       <c r="B160">
         <v>1.381619305127595</v>
@@ -8285,7 +8285,7 @@
     </row>
     <row r="161">
       <c r="A161" s="2">
-        <v>44295.04166666667</v>
+        <v>44295.66666666667</v>
       </c>
       <c r="B161">
         <v>1.675415639473132</v>
@@ -8336,7 +8336,7 @@
     </row>
     <row r="162">
       <c r="A162" s="2">
-        <v>44295.08333333333</v>
+        <v>44295.70833333333</v>
       </c>
       <c r="B162">
         <v>1.668828277716511</v>
@@ -8387,10 +8387,10 @@
     </row>
     <row r="163">
       <c r="A163" s="2">
-        <v>44295.125</v>
+        <v>44295.75</v>
       </c>
       <c r="B163">
-        <v>1.782130899930482</v>
+        <v>1.782130899930481</v>
       </c>
       <c r="C163" s="3">
         <v>44295</v>
@@ -8438,7 +8438,7 @@
     </row>
     <row r="164">
       <c r="A164" s="2">
-        <v>44295.16666666667</v>
+        <v>44295.79166666667</v>
       </c>
       <c r="B164">
         <v>1.950767360900124</v>
@@ -8489,7 +8489,7 @@
     </row>
     <row r="165">
       <c r="A165" s="2">
-        <v>44295.20833333333</v>
+        <v>44295.83333333333</v>
       </c>
       <c r="B165">
         <v>1.956037250305428</v>
@@ -8518,7 +8518,7 @@
         <v>62</v>
       </c>
       <c r="J165">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K165">
         <v>223</v>
@@ -8540,7 +8540,7 @@
     </row>
     <row r="166">
       <c r="A166" s="2">
-        <v>44295.25</v>
+        <v>44295.875</v>
       </c>
       <c r="B166">
         <v>2.07724470662735</v>
@@ -8591,10 +8591,10 @@
     </row>
     <row r="167">
       <c r="A167" s="2">
-        <v>44295.29166666667</v>
+        <v>44295.91666666667</v>
       </c>
       <c r="B167">
-        <v>2.197134690597956</v>
+        <v>2.197134690597955</v>
       </c>
       <c r="C167" s="3">
         <v>44295</v>
@@ -8642,7 +8642,7 @@
     </row>
     <row r="168">
       <c r="A168" s="2">
-        <v>44295.33333333333</v>
+        <v>44295.95833333333</v>
       </c>
       <c r="B168">
         <v>2.177372605328072</v>
@@ -8693,10 +8693,10 @@
     </row>
     <row r="169">
       <c r="A169" s="2">
-        <v>44295.375</v>
+        <v>44296</v>
       </c>
       <c r="B169">
-        <v>2.18791238413868</v>
+        <v>2.187912384138679</v>
       </c>
       <c r="C169" s="3">
         <v>44295</v>
@@ -8744,10 +8744,10 @@
     </row>
     <row r="170">
       <c r="A170" s="2">
-        <v>44295.41666666667</v>
+        <v>44296.04166666667</v>
       </c>
       <c r="B170">
-        <v>2.166832826517472</v>
+        <v>2.166832826517471</v>
       </c>
       <c r="C170" s="3">
         <v>44295</v>
@@ -8795,10 +8795,10 @@
     </row>
     <row r="171">
       <c r="A171" s="2">
-        <v>44295.45833333333</v>
+        <v>44296.08333333333</v>
       </c>
       <c r="B171">
-        <v>2.197134690597956</v>
+        <v>2.197134690597955</v>
       </c>
       <c r="C171" s="3">
         <v>44295</v>
@@ -8816,7 +8816,7 @@
     </row>
     <row r="172">
       <c r="A172" s="2">
-        <v>44281.5</v>
+        <v>44282.125</v>
       </c>
       <c r="C172" s="3">
         <v>44281</v>
@@ -8864,7 +8864,7 @@
     </row>
     <row r="173">
       <c r="A173" s="2">
-        <v>44281.54166666667</v>
+        <v>44282.16666666667</v>
       </c>
       <c r="C173" s="3">
         <v>44281</v>
@@ -8912,7 +8912,7 @@
     </row>
     <row r="174">
       <c r="A174" s="2">
-        <v>44281.58333333333</v>
+        <v>44282.20833333333</v>
       </c>
       <c r="C174" s="3">
         <v>44281</v>
@@ -8960,7 +8960,7 @@
     </row>
     <row r="175">
       <c r="A175" s="2">
-        <v>44281.625</v>
+        <v>44282.25</v>
       </c>
       <c r="C175" s="3">
         <v>44281</v>
@@ -9008,7 +9008,7 @@
     </row>
     <row r="176">
       <c r="A176" s="2">
-        <v>44281.66666666667</v>
+        <v>44282.29166666667</v>
       </c>
       <c r="C176" s="3">
         <v>44282</v>
@@ -9056,7 +9056,7 @@
     </row>
     <row r="177">
       <c r="A177" s="2">
-        <v>44281.70833333333</v>
+        <v>44282.33333333333</v>
       </c>
       <c r="C177" s="3">
         <v>44282</v>
@@ -9104,7 +9104,7 @@
     </row>
     <row r="178">
       <c r="A178" s="2">
-        <v>44281.75</v>
+        <v>44282.375</v>
       </c>
       <c r="C178" s="3">
         <v>44282</v>
@@ -9152,7 +9152,7 @@
     </row>
     <row r="179">
       <c r="A179" s="2">
-        <v>44281.79166666667</v>
+        <v>44282.41666666667</v>
       </c>
       <c r="C179" s="3">
         <v>44282</v>
@@ -9200,7 +9200,7 @@
     </row>
     <row r="180">
       <c r="A180" s="2">
-        <v>44281.83333333333</v>
+        <v>44282.45833333333</v>
       </c>
       <c r="C180" s="3">
         <v>44282</v>
@@ -9248,7 +9248,7 @@
     </row>
     <row r="181">
       <c r="A181" s="2">
-        <v>44281.875</v>
+        <v>44282.5</v>
       </c>
       <c r="C181" s="3">
         <v>44282</v>
@@ -9296,7 +9296,7 @@
     </row>
     <row r="182">
       <c r="A182" s="2">
-        <v>44281.91666666667</v>
+        <v>44282.54166666667</v>
       </c>
       <c r="C182" s="3">
         <v>44282</v>
@@ -9344,7 +9344,7 @@
     </row>
     <row r="183">
       <c r="A183" s="2">
-        <v>44281.95833333333</v>
+        <v>44282.58333333333</v>
       </c>
       <c r="C183" s="3">
         <v>44282</v>
@@ -9392,7 +9392,7 @@
     </row>
     <row r="184">
       <c r="A184" s="2">
-        <v>44282</v>
+        <v>44282.625</v>
       </c>
       <c r="C184" s="3">
         <v>44282</v>
@@ -9440,7 +9440,7 @@
     </row>
     <row r="185">
       <c r="A185" s="2">
-        <v>44282.04166666667</v>
+        <v>44282.66666666667</v>
       </c>
       <c r="C185" s="3">
         <v>44282</v>
@@ -9488,7 +9488,7 @@
     </row>
     <row r="186">
       <c r="A186" s="2">
-        <v>44282.08333333333</v>
+        <v>44282.70833333333</v>
       </c>
       <c r="C186" s="3">
         <v>44282</v>
@@ -9536,7 +9536,7 @@
     </row>
     <row r="187">
       <c r="A187" s="2">
-        <v>44282.125</v>
+        <v>44282.75</v>
       </c>
       <c r="C187" s="3">
         <v>44282</v>
@@ -9584,7 +9584,7 @@
     </row>
     <row r="188">
       <c r="A188" s="2">
-        <v>44282.16666666667</v>
+        <v>44282.79166666667</v>
       </c>
       <c r="C188" s="3">
         <v>44282</v>
@@ -9632,7 +9632,7 @@
     </row>
     <row r="189">
       <c r="A189" s="2">
-        <v>44282.20833333333</v>
+        <v>44282.83333333333</v>
       </c>
       <c r="C189" s="3">
         <v>44282</v>
@@ -9680,7 +9680,7 @@
     </row>
     <row r="190">
       <c r="A190" s="2">
-        <v>44282.25</v>
+        <v>44282.875</v>
       </c>
       <c r="C190" s="3">
         <v>44282</v>
@@ -9728,7 +9728,7 @@
     </row>
     <row r="191">
       <c r="A191" s="2">
-        <v>44282.29166666667</v>
+        <v>44282.91666666667</v>
       </c>
       <c r="C191" s="3">
         <v>44282</v>
@@ -9776,7 +9776,7 @@
     </row>
     <row r="192">
       <c r="A192" s="2">
-        <v>44282.33333333333</v>
+        <v>44282.95833333333</v>
       </c>
       <c r="C192" s="3">
         <v>44282</v>
@@ -9824,7 +9824,7 @@
     </row>
     <row r="193">
       <c r="A193" s="2">
-        <v>44282.375</v>
+        <v>44283</v>
       </c>
       <c r="C193" s="3">
         <v>44282</v>
@@ -9872,7 +9872,7 @@
     </row>
     <row r="194">
       <c r="A194" s="2">
-        <v>44282.41666666667</v>
+        <v>44283.04166666667</v>
       </c>
       <c r="C194" s="3">
         <v>44282</v>
@@ -9920,7 +9920,7 @@
     </row>
     <row r="195">
       <c r="A195" s="2">
-        <v>44282.45833333333</v>
+        <v>44283.08333333333</v>
       </c>
       <c r="C195" s="3">
         <v>44282</v>
@@ -9968,7 +9968,7 @@
     </row>
     <row r="196">
       <c r="A196" s="2">
-        <v>44282.5</v>
+        <v>44283.125</v>
       </c>
       <c r="C196" s="3">
         <v>44282</v>
@@ -10016,7 +10016,7 @@
     </row>
     <row r="197">
       <c r="A197" s="2">
-        <v>44282.54166666667</v>
+        <v>44283.16666666667</v>
       </c>
       <c r="C197" s="3">
         <v>44282</v>
@@ -10064,7 +10064,7 @@
     </row>
     <row r="198">
       <c r="A198" s="2">
-        <v>44282.58333333333</v>
+        <v>44283.20833333333</v>
       </c>
       <c r="C198" s="3">
         <v>44282</v>
@@ -10112,7 +10112,7 @@
     </row>
     <row r="199">
       <c r="A199" s="2">
-        <v>44282.625</v>
+        <v>44283.25</v>
       </c>
       <c r="C199" s="3">
         <v>44282</v>
@@ -10160,7 +10160,7 @@
     </row>
     <row r="200">
       <c r="A200" s="2">
-        <v>44282.66666666667</v>
+        <v>44283.29166666667</v>
       </c>
       <c r="C200" s="3">
         <v>44283</v>
@@ -10208,7 +10208,7 @@
     </row>
     <row r="201">
       <c r="A201" s="2">
-        <v>44282.70833333333</v>
+        <v>44283.33333333333</v>
       </c>
       <c r="C201" s="3">
         <v>44283</v>
@@ -10256,7 +10256,7 @@
     </row>
     <row r="202">
       <c r="A202" s="2">
-        <v>44282.75</v>
+        <v>44283.375</v>
       </c>
       <c r="C202" s="3">
         <v>44283</v>
@@ -10304,7 +10304,7 @@
     </row>
     <row r="203">
       <c r="A203" s="2">
-        <v>44282.79166666667</v>
+        <v>44283.41666666667</v>
       </c>
       <c r="C203" s="3">
         <v>44283</v>
@@ -10352,7 +10352,7 @@
     </row>
     <row r="204">
       <c r="A204" s="2">
-        <v>44282.83333333333</v>
+        <v>44283.45833333333</v>
       </c>
       <c r="C204" s="3">
         <v>44283</v>
@@ -10400,7 +10400,7 @@
     </row>
     <row r="205">
       <c r="A205" s="2">
-        <v>44282.875</v>
+        <v>44283.5</v>
       </c>
       <c r="C205" s="3">
         <v>44283</v>
@@ -10448,7 +10448,7 @@
     </row>
     <row r="206">
       <c r="A206" s="2">
-        <v>44282.91666666667</v>
+        <v>44283.54166666667</v>
       </c>
       <c r="C206" s="3">
         <v>44283</v>
@@ -10496,7 +10496,7 @@
     </row>
     <row r="207">
       <c r="A207" s="2">
-        <v>44282.95833333333</v>
+        <v>44283.58333333333</v>
       </c>
       <c r="C207" s="3">
         <v>44283</v>
@@ -10544,7 +10544,7 @@
     </row>
     <row r="208">
       <c r="A208" s="2">
-        <v>44283</v>
+        <v>44283.625</v>
       </c>
       <c r="C208" s="3">
         <v>44283</v>
@@ -10592,7 +10592,7 @@
     </row>
     <row r="209">
       <c r="A209" s="2">
-        <v>44283.04166666667</v>
+        <v>44283.66666666667</v>
       </c>
       <c r="C209" s="3">
         <v>44283</v>
@@ -10640,7 +10640,7 @@
     </row>
     <row r="210">
       <c r="A210" s="2">
-        <v>44283.08333333333</v>
+        <v>44283.70833333333</v>
       </c>
       <c r="C210" s="3">
         <v>44283</v>
@@ -10688,7 +10688,7 @@
     </row>
     <row r="211">
       <c r="A211" s="2">
-        <v>44283.125</v>
+        <v>44283.75</v>
       </c>
       <c r="C211" s="3">
         <v>44283</v>
@@ -10736,7 +10736,7 @@
     </row>
     <row r="212">
       <c r="A212" s="2">
-        <v>44283.16666666667</v>
+        <v>44283.79166666667</v>
       </c>
       <c r="C212" s="3">
         <v>44283</v>
@@ -10784,7 +10784,7 @@
     </row>
     <row r="213">
       <c r="A213" s="2">
-        <v>44283.20833333333</v>
+        <v>44283.83333333333</v>
       </c>
       <c r="C213" s="3">
         <v>44283</v>
@@ -10832,7 +10832,7 @@
     </row>
     <row r="214">
       <c r="A214" s="2">
-        <v>44283.25</v>
+        <v>44283.875</v>
       </c>
       <c r="C214" s="3">
         <v>44283</v>
@@ -10880,7 +10880,7 @@
     </row>
     <row r="215">
       <c r="A215" s="2">
-        <v>44283.29166666667</v>
+        <v>44283.91666666667</v>
       </c>
       <c r="C215" s="3">
         <v>44283</v>
@@ -10928,7 +10928,7 @@
     </row>
     <row r="216">
       <c r="A216" s="2">
-        <v>44283.33333333333</v>
+        <v>44283.95833333333</v>
       </c>
       <c r="C216" s="3">
         <v>44283</v>
@@ -10976,7 +10976,7 @@
     </row>
     <row r="217">
       <c r="A217" s="2">
-        <v>44283.375</v>
+        <v>44284</v>
       </c>
       <c r="C217" s="3">
         <v>44283</v>
@@ -11024,7 +11024,7 @@
     </row>
     <row r="218">
       <c r="A218" s="2">
-        <v>44283.41666666667</v>
+        <v>44284.04166666667</v>
       </c>
       <c r="C218" s="3">
         <v>44283</v>
@@ -11072,7 +11072,7 @@
     </row>
     <row r="219">
       <c r="A219" s="2">
-        <v>44283.45833333333</v>
+        <v>44284.08333333333</v>
       </c>
       <c r="C219" s="3">
         <v>44283</v>
@@ -11120,7 +11120,7 @@
     </row>
     <row r="220">
       <c r="A220" s="2">
-        <v>44283.5</v>
+        <v>44284.125</v>
       </c>
       <c r="C220" s="3">
         <v>44283</v>
@@ -11168,7 +11168,7 @@
     </row>
     <row r="221">
       <c r="A221" s="2">
-        <v>44283.54166666667</v>
+        <v>44284.16666666667</v>
       </c>
       <c r="C221" s="3">
         <v>44283</v>
@@ -11216,7 +11216,7 @@
     </row>
     <row r="222">
       <c r="A222" s="2">
-        <v>44283.58333333333</v>
+        <v>44284.20833333333</v>
       </c>
       <c r="C222" s="3">
         <v>44283</v>
@@ -11264,7 +11264,7 @@
     </row>
     <row r="223">
       <c r="A223" s="2">
-        <v>44283.625</v>
+        <v>44284.25</v>
       </c>
       <c r="C223" s="3">
         <v>44283</v>
@@ -11312,7 +11312,7 @@
     </row>
     <row r="224">
       <c r="A224" s="2">
-        <v>44283.66666666667</v>
+        <v>44284.29166666667</v>
       </c>
       <c r="C224" s="3">
         <v>44284</v>
@@ -11360,7 +11360,7 @@
     </row>
     <row r="225">
       <c r="A225" s="2">
-        <v>44283.70833333333</v>
+        <v>44284.33333333333</v>
       </c>
       <c r="C225" s="3">
         <v>44284</v>
@@ -11408,7 +11408,7 @@
     </row>
     <row r="226">
       <c r="A226" s="2">
-        <v>44283.75</v>
+        <v>44284.375</v>
       </c>
       <c r="C226" s="3">
         <v>44284</v>
@@ -11456,7 +11456,7 @@
     </row>
     <row r="227">
       <c r="A227" s="2">
-        <v>44284.5</v>
+        <v>44285.125</v>
       </c>
       <c r="C227" s="3">
         <v>44284</v>
@@ -11504,7 +11504,7 @@
     </row>
     <row r="228">
       <c r="A228" s="2">
-        <v>44284.54166666667</v>
+        <v>44285.16666666667</v>
       </c>
       <c r="C228" s="3">
         <v>44284</v>
@@ -11552,7 +11552,7 @@
     </row>
     <row r="229">
       <c r="A229" s="2">
-        <v>44284.58333333333</v>
+        <v>44285.20833333333</v>
       </c>
       <c r="C229" s="3">
         <v>44284</v>
@@ -11600,7 +11600,7 @@
     </row>
     <row r="230">
       <c r="A230" s="2">
-        <v>44284.625</v>
+        <v>44285.25</v>
       </c>
       <c r="C230" s="3">
         <v>44284</v>
@@ -11648,7 +11648,7 @@
     </row>
     <row r="231">
       <c r="A231" s="2">
-        <v>44284.66666666667</v>
+        <v>44285.29166666667</v>
       </c>
       <c r="C231" s="3">
         <v>44285</v>
@@ -11696,7 +11696,7 @@
     </row>
     <row r="232">
       <c r="A232" s="2">
-        <v>44284.70833333333</v>
+        <v>44285.33333333333</v>
       </c>
       <c r="C232" s="3">
         <v>44285</v>
@@ -11744,7 +11744,7 @@
     </row>
     <row r="233">
       <c r="A233" s="2">
-        <v>44284.75</v>
+        <v>44285.375</v>
       </c>
       <c r="C233" s="3">
         <v>44285</v>
@@ -11792,7 +11792,7 @@
     </row>
     <row r="234">
       <c r="A234" s="2">
-        <v>44285.5</v>
+        <v>44286.125</v>
       </c>
       <c r="C234" s="3">
         <v>44285</v>
@@ -11840,7 +11840,7 @@
     </row>
     <row r="235">
       <c r="A235" s="2">
-        <v>44285.54166666667</v>
+        <v>44286.16666666667</v>
       </c>
       <c r="C235" s="3">
         <v>44285</v>
@@ -11888,7 +11888,7 @@
     </row>
     <row r="236">
       <c r="A236" s="2">
-        <v>44285.58333333333</v>
+        <v>44286.20833333333</v>
       </c>
       <c r="C236" s="3">
         <v>44285</v>
@@ -11936,7 +11936,7 @@
     </row>
     <row r="237">
       <c r="A237" s="2">
-        <v>44285.625</v>
+        <v>44286.25</v>
       </c>
       <c r="C237" s="3">
         <v>44285</v>
@@ -11984,7 +11984,7 @@
     </row>
     <row r="238">
       <c r="A238" s="2">
-        <v>44285.66666666667</v>
+        <v>44286.29166666667</v>
       </c>
       <c r="C238" s="3">
         <v>44286</v>
@@ -12032,7 +12032,7 @@
     </row>
     <row r="239">
       <c r="A239" s="2">
-        <v>44285.70833333333</v>
+        <v>44286.33333333333</v>
       </c>
       <c r="C239" s="3">
         <v>44286</v>
@@ -12080,7 +12080,7 @@
     </row>
     <row r="240">
       <c r="A240" s="2">
-        <v>44285.75</v>
+        <v>44286.375</v>
       </c>
       <c r="C240" s="3">
         <v>44286</v>
@@ -12128,7 +12128,7 @@
     </row>
     <row r="241">
       <c r="A241" s="2">
-        <v>44286.5</v>
+        <v>44287.125</v>
       </c>
       <c r="C241" s="3">
         <v>44286</v>
@@ -12176,7 +12176,7 @@
     </row>
     <row r="242">
       <c r="A242" s="2">
-        <v>44286.54166666667</v>
+        <v>44287.16666666667</v>
       </c>
       <c r="C242" s="3">
         <v>44286</v>
@@ -12224,7 +12224,7 @@
     </row>
     <row r="243">
       <c r="A243" s="2">
-        <v>44286.58333333333</v>
+        <v>44287.20833333333</v>
       </c>
       <c r="C243" s="3">
         <v>44286</v>
@@ -12272,7 +12272,7 @@
     </row>
     <row r="244">
       <c r="A244" s="2">
-        <v>44286.625</v>
+        <v>44287.25</v>
       </c>
       <c r="C244" s="3">
         <v>44286</v>
@@ -12320,7 +12320,7 @@
     </row>
     <row r="245">
       <c r="A245" s="2">
-        <v>44286.66666666667</v>
+        <v>44287.29166666667</v>
       </c>
       <c r="C245" s="3">
         <v>44287</v>
@@ -12368,7 +12368,7 @@
     </row>
     <row r="246">
       <c r="A246" s="2">
-        <v>44286.70833333333</v>
+        <v>44287.33333333333</v>
       </c>
       <c r="C246" s="3">
         <v>44287</v>
@@ -12416,7 +12416,7 @@
     </row>
     <row r="247">
       <c r="A247" s="2">
-        <v>44286.75</v>
+        <v>44287.375</v>
       </c>
       <c r="C247" s="3">
         <v>44287</v>
@@ -12464,7 +12464,7 @@
     </row>
     <row r="248">
       <c r="A248" s="2">
-        <v>44287.5</v>
+        <v>44288.125</v>
       </c>
       <c r="C248" s="3">
         <v>44287</v>
@@ -12512,7 +12512,7 @@
     </row>
     <row r="249">
       <c r="A249" s="2">
-        <v>44287.54166666667</v>
+        <v>44288.16666666667</v>
       </c>
       <c r="C249" s="3">
         <v>44287</v>
@@ -12560,7 +12560,7 @@
     </row>
     <row r="250">
       <c r="A250" s="2">
-        <v>44287.58333333333</v>
+        <v>44288.20833333333</v>
       </c>
       <c r="C250" s="3">
         <v>44287</v>
@@ -12608,7 +12608,7 @@
     </row>
     <row r="251">
       <c r="A251" s="2">
-        <v>44287.625</v>
+        <v>44288.25</v>
       </c>
       <c r="C251" s="3">
         <v>44287</v>
@@ -12656,7 +12656,7 @@
     </row>
     <row r="252">
       <c r="A252" s="2">
-        <v>44287.66666666667</v>
+        <v>44288.29166666667</v>
       </c>
       <c r="C252" s="3">
         <v>44288</v>
@@ -12704,7 +12704,7 @@
     </row>
     <row r="253">
       <c r="A253" s="2">
-        <v>44287.70833333333</v>
+        <v>44288.33333333333</v>
       </c>
       <c r="C253" s="3">
         <v>44288</v>
@@ -12752,7 +12752,7 @@
     </row>
     <row r="254">
       <c r="A254" s="2">
-        <v>44287.75</v>
+        <v>44288.375</v>
       </c>
       <c r="C254" s="3">
         <v>44288</v>
@@ -12800,7 +12800,7 @@
     </row>
     <row r="255">
       <c r="A255" s="2">
-        <v>44287.79166666667</v>
+        <v>44288.41666666667</v>
       </c>
       <c r="C255" s="3">
         <v>44288</v>
@@ -12848,7 +12848,7 @@
     </row>
     <row r="256">
       <c r="A256" s="2">
-        <v>44287.83333333333</v>
+        <v>44288.45833333333</v>
       </c>
       <c r="C256" s="3">
         <v>44288</v>
@@ -12896,7 +12896,7 @@
     </row>
     <row r="257">
       <c r="A257" s="2">
-        <v>44287.875</v>
+        <v>44288.5</v>
       </c>
       <c r="C257" s="3">
         <v>44288</v>
@@ -12944,7 +12944,7 @@
     </row>
     <row r="258">
       <c r="A258" s="2">
-        <v>44287.91666666667</v>
+        <v>44288.54166666667</v>
       </c>
       <c r="C258" s="3">
         <v>44288</v>
@@ -12992,7 +12992,7 @@
     </row>
     <row r="259">
       <c r="A259" s="2">
-        <v>44287.95833333333</v>
+        <v>44288.58333333333</v>
       </c>
       <c r="C259" s="3">
         <v>44288</v>
@@ -13040,7 +13040,7 @@
     </row>
     <row r="260">
       <c r="A260" s="2">
-        <v>44288</v>
+        <v>44288.625</v>
       </c>
       <c r="C260" s="3">
         <v>44288</v>
@@ -13088,7 +13088,7 @@
     </row>
     <row r="261">
       <c r="A261" s="2">
-        <v>44288.04166666667</v>
+        <v>44288.66666666667</v>
       </c>
       <c r="C261" s="3">
         <v>44288</v>
@@ -13136,7 +13136,7 @@
     </row>
     <row r="262">
       <c r="A262" s="2">
-        <v>44288.08333333333</v>
+        <v>44288.70833333333</v>
       </c>
       <c r="C262" s="3">
         <v>44288</v>
@@ -13184,7 +13184,7 @@
     </row>
     <row r="263">
       <c r="A263" s="2">
-        <v>44288.125</v>
+        <v>44288.75</v>
       </c>
       <c r="C263" s="3">
         <v>44288</v>
@@ -13232,7 +13232,7 @@
     </row>
     <row r="264">
       <c r="A264" s="2">
-        <v>44288.16666666667</v>
+        <v>44288.79166666667</v>
       </c>
       <c r="C264" s="3">
         <v>44288</v>
@@ -13280,7 +13280,7 @@
     </row>
     <row r="265">
       <c r="A265" s="2">
-        <v>44288.20833333333</v>
+        <v>44288.83333333333</v>
       </c>
       <c r="C265" s="3">
         <v>44288</v>
@@ -13328,7 +13328,7 @@
     </row>
     <row r="266">
       <c r="A266" s="2">
-        <v>44288.25</v>
+        <v>44288.875</v>
       </c>
       <c r="C266" s="3">
         <v>44288</v>
@@ -13376,7 +13376,7 @@
     </row>
     <row r="267">
       <c r="A267" s="2">
-        <v>44288.29166666667</v>
+        <v>44288.91666666667</v>
       </c>
       <c r="C267" s="3">
         <v>44288</v>
@@ -13424,7 +13424,7 @@
     </row>
     <row r="268">
       <c r="A268" s="2">
-        <v>44288.33333333333</v>
+        <v>44288.95833333333</v>
       </c>
       <c r="C268" s="3">
         <v>44288</v>
@@ -13472,7 +13472,7 @@
     </row>
     <row r="269">
       <c r="A269" s="2">
-        <v>44288.375</v>
+        <v>44289</v>
       </c>
       <c r="C269" s="3">
         <v>44288</v>
@@ -13520,7 +13520,7 @@
     </row>
     <row r="270">
       <c r="A270" s="2">
-        <v>44288.41666666667</v>
+        <v>44289.04166666667</v>
       </c>
       <c r="C270" s="3">
         <v>44288</v>
@@ -13568,7 +13568,7 @@
     </row>
     <row r="271">
       <c r="A271" s="2">
-        <v>44288.45833333333</v>
+        <v>44289.08333333333</v>
       </c>
       <c r="C271" s="3">
         <v>44288</v>
@@ -13616,7 +13616,7 @@
     </row>
     <row r="272">
       <c r="A272" s="2">
-        <v>44288.5</v>
+        <v>44289.125</v>
       </c>
       <c r="C272" s="3">
         <v>44288</v>
@@ -13664,7 +13664,7 @@
     </row>
     <row r="273">
       <c r="A273" s="2">
-        <v>44288.54166666667</v>
+        <v>44289.16666666667</v>
       </c>
       <c r="C273" s="3">
         <v>44288</v>
@@ -13712,7 +13712,7 @@
     </row>
     <row r="274">
       <c r="A274" s="2">
-        <v>44288.58333333333</v>
+        <v>44289.20833333333</v>
       </c>
       <c r="C274" s="3">
         <v>44288</v>
@@ -13760,7 +13760,7 @@
     </row>
     <row r="275">
       <c r="A275" s="2">
-        <v>44290.33333333333</v>
+        <v>44290.95833333333</v>
       </c>
       <c r="C275" s="3">
         <v>44290</v>
@@ -13808,7 +13808,7 @@
     </row>
     <row r="276">
       <c r="A276" s="2">
-        <v>44290.375</v>
+        <v>44291</v>
       </c>
       <c r="C276" s="3">
         <v>44290</v>
@@ -13856,7 +13856,7 @@
     </row>
     <row r="277">
       <c r="A277" s="2">
-        <v>44290.41666666667</v>
+        <v>44291.04166666667</v>
       </c>
       <c r="C277" s="3">
         <v>44290</v>
@@ -13904,7 +13904,7 @@
     </row>
     <row r="278">
       <c r="A278" s="2">
-        <v>44290.45833333333</v>
+        <v>44291.08333333333</v>
       </c>
       <c r="C278" s="3">
         <v>44290</v>
@@ -13952,7 +13952,7 @@
     </row>
     <row r="279">
       <c r="A279" s="2">
-        <v>44290.5</v>
+        <v>44291.125</v>
       </c>
       <c r="C279" s="3">
         <v>44290</v>
@@ -14000,7 +14000,7 @@
     </row>
     <row r="280">
       <c r="A280" s="2">
-        <v>44290.54166666667</v>
+        <v>44291.16666666667</v>
       </c>
       <c r="C280" s="3">
         <v>44290</v>
@@ -14048,7 +14048,7 @@
     </row>
     <row r="281">
       <c r="A281" s="2">
-        <v>44290.58333333333</v>
+        <v>44291.20833333333</v>
       </c>
       <c r="C281" s="3">
         <v>44290</v>
@@ -14096,7 +14096,7 @@
     </row>
     <row r="282">
       <c r="A282" s="2">
-        <v>44290.625</v>
+        <v>44291.25</v>
       </c>
       <c r="C282" s="3">
         <v>44290</v>
@@ -14144,7 +14144,7 @@
     </row>
     <row r="283">
       <c r="A283" s="2">
-        <v>44290.66666666667</v>
+        <v>44291.29166666667</v>
       </c>
       <c r="C283" s="3">
         <v>44291</v>
@@ -14192,7 +14192,7 @@
     </row>
     <row r="284">
       <c r="A284" s="2">
-        <v>44290.70833333333</v>
+        <v>44291.33333333333</v>
       </c>
       <c r="C284" s="3">
         <v>44291</v>
@@ -14240,7 +14240,7 @@
     </row>
     <row r="285">
       <c r="A285" s="2">
-        <v>44290.75</v>
+        <v>44291.375</v>
       </c>
       <c r="C285" s="3">
         <v>44291</v>
@@ -14288,7 +14288,7 @@
     </row>
     <row r="286">
       <c r="A286" s="2">
-        <v>44291.5</v>
+        <v>44292.125</v>
       </c>
       <c r="C286" s="3">
         <v>44291</v>
@@ -14336,7 +14336,7 @@
     </row>
     <row r="287">
       <c r="A287" s="2">
-        <v>44291.54166666667</v>
+        <v>44292.16666666667</v>
       </c>
       <c r="C287" s="3">
         <v>44291</v>
@@ -14384,7 +14384,7 @@
     </row>
     <row r="288">
       <c r="A288" s="2">
-        <v>44291.58333333333</v>
+        <v>44292.20833333333</v>
       </c>
       <c r="C288" s="3">
         <v>44291</v>
@@ -14432,7 +14432,7 @@
     </row>
     <row r="289">
       <c r="A289" s="2">
-        <v>44291.625</v>
+        <v>44292.25</v>
       </c>
       <c r="C289" s="3">
         <v>44291</v>
@@ -14480,7 +14480,7 @@
     </row>
     <row r="290">
       <c r="A290" s="2">
-        <v>44291.66666666667</v>
+        <v>44292.29166666667</v>
       </c>
       <c r="C290" s="3">
         <v>44292</v>
@@ -14528,7 +14528,7 @@
     </row>
     <row r="291">
       <c r="A291" s="2">
-        <v>44291.70833333333</v>
+        <v>44292.33333333333</v>
       </c>
       <c r="C291" s="3">
         <v>44292</v>
@@ -14576,7 +14576,7 @@
     </row>
     <row r="292">
       <c r="A292" s="2">
-        <v>44291.75</v>
+        <v>44292.375</v>
       </c>
       <c r="C292" s="3">
         <v>44292</v>
@@ -14624,7 +14624,7 @@
     </row>
     <row r="293">
       <c r="A293" s="2">
-        <v>44292.5</v>
+        <v>44293.125</v>
       </c>
       <c r="C293" s="3">
         <v>44292</v>
@@ -14672,7 +14672,7 @@
     </row>
     <row r="294">
       <c r="A294" s="2">
-        <v>44292.54166666667</v>
+        <v>44293.16666666667</v>
       </c>
       <c r="C294" s="3">
         <v>44292</v>
@@ -14720,7 +14720,7 @@
     </row>
     <row r="295">
       <c r="A295" s="2">
-        <v>44292.58333333333</v>
+        <v>44293.20833333333</v>
       </c>
       <c r="C295" s="3">
         <v>44292</v>
@@ -14768,7 +14768,7 @@
     </row>
     <row r="296">
       <c r="A296" s="2">
-        <v>44292.625</v>
+        <v>44293.25</v>
       </c>
       <c r="C296" s="3">
         <v>44292</v>
@@ -14816,7 +14816,7 @@
     </row>
     <row r="297">
       <c r="A297" s="2">
-        <v>44292.66666666667</v>
+        <v>44293.29166666667</v>
       </c>
       <c r="C297" s="3">
         <v>44293</v>
@@ -14864,7 +14864,7 @@
     </row>
     <row r="298">
       <c r="A298" s="2">
-        <v>44292.70833333333</v>
+        <v>44293.33333333333</v>
       </c>
       <c r="C298" s="3">
         <v>44293</v>
@@ -14912,7 +14912,7 @@
     </row>
     <row r="299">
       <c r="A299" s="2">
-        <v>44292.75</v>
+        <v>44293.375</v>
       </c>
       <c r="C299" s="3">
         <v>44293</v>
@@ -14960,7 +14960,7 @@
     </row>
     <row r="300">
       <c r="A300" s="2">
-        <v>44293.5</v>
+        <v>44294.125</v>
       </c>
       <c r="C300" s="3">
         <v>44293</v>
@@ -15008,7 +15008,7 @@
     </row>
     <row r="301">
       <c r="A301" s="2">
-        <v>44293.54166666667</v>
+        <v>44294.16666666667</v>
       </c>
       <c r="C301" s="3">
         <v>44293</v>
@@ -15056,7 +15056,7 @@
     </row>
     <row r="302">
       <c r="A302" s="2">
-        <v>44293.58333333333</v>
+        <v>44294.20833333333</v>
       </c>
       <c r="C302" s="3">
         <v>44293</v>
@@ -15104,7 +15104,7 @@
     </row>
     <row r="303">
       <c r="A303" s="2">
-        <v>44293.625</v>
+        <v>44294.25</v>
       </c>
       <c r="C303" s="3">
         <v>44293</v>
@@ -15152,7 +15152,7 @@
     </row>
     <row r="304">
       <c r="A304" s="2">
-        <v>44293.66666666667</v>
+        <v>44294.29166666667</v>
       </c>
       <c r="C304" s="3">
         <v>44294</v>
@@ -15200,7 +15200,7 @@
     </row>
     <row r="305">
       <c r="A305" s="2">
-        <v>44293.70833333333</v>
+        <v>44294.33333333333</v>
       </c>
       <c r="C305" s="3">
         <v>44294</v>
@@ -15248,7 +15248,7 @@
     </row>
     <row r="306">
       <c r="A306" s="2">
-        <v>44293.75</v>
+        <v>44294.375</v>
       </c>
       <c r="C306" s="3">
         <v>44294</v>
@@ -15296,7 +15296,7 @@
     </row>
     <row r="307">
       <c r="A307" s="2">
-        <v>44294.5</v>
+        <v>44295.125</v>
       </c>
       <c r="C307" s="3">
         <v>44294</v>
@@ -15344,7 +15344,7 @@
     </row>
     <row r="308">
       <c r="A308" s="2">
-        <v>44294.54166666667</v>
+        <v>44295.16666666667</v>
       </c>
       <c r="C308" s="3">
         <v>44294</v>
@@ -15392,7 +15392,7 @@
     </row>
     <row r="309">
       <c r="A309" s="2">
-        <v>44294.58333333333</v>
+        <v>44295.20833333333</v>
       </c>
       <c r="C309" s="3">
         <v>44294</v>
@@ -15440,7 +15440,7 @@
     </row>
     <row r="310">
       <c r="A310" s="2">
-        <v>44294.625</v>
+        <v>44295.25</v>
       </c>
       <c r="C310" s="3">
         <v>44294</v>
@@ -15488,7 +15488,7 @@
     </row>
     <row r="311">
       <c r="A311" s="2">
-        <v>44294.66666666667</v>
+        <v>44295.29166666667</v>
       </c>
       <c r="C311" s="3">
         <v>44295</v>
@@ -15536,7 +15536,7 @@
     </row>
     <row r="312">
       <c r="A312" s="2">
-        <v>44294.70833333333</v>
+        <v>44295.33333333333</v>
       </c>
       <c r="C312" s="3">
         <v>44295</v>
@@ -15584,7 +15584,7 @@
     </row>
     <row r="313">
       <c r="A313" s="2">
-        <v>44294.75</v>
+        <v>44295.375</v>
       </c>
       <c r="C313" s="3">
         <v>44295</v>

</xml_diff>